<commit_message>
Thank you Bradley for organising this.
</commit_message>
<xml_diff>
--- a/leaftop-evaluations/hmo.xlsx
+++ b/leaftop-evaluations/hmo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maureen\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gregb/Documents/devel/phd/thousand-language-morphology/leaftop-evaluations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13D4A6D9-07E7-4EFA-95F3-7ECCF97D7155}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{633ACF36-A03F-C947-812D-E64FF94F1971}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19400" windowHeight="10400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3536" uniqueCount="598">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3539" uniqueCount="598">
   <si>
     <t>lemma</t>
   </si>
@@ -2232,19 +2232,19 @@
   <dimension ref="A1:K393"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K394" sqref="K394"/>
+      <pane ySplit="1" topLeftCell="A216" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K219" sqref="K219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="7" max="7" width="8.83984375" customWidth="1"/>
-    <col min="9" max="9" width="22.578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="46.41796875" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" customWidth="1"/>
+    <col min="9" max="9" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="46.5" customWidth="1"/>
     <col min="11" max="11" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2279,7 +2279,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -2314,7 +2314,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>10</v>
       </c>
@@ -2349,7 +2349,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2384,7 +2384,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -2454,7 +2454,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2489,7 +2489,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2524,7 +2524,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -2559,7 +2559,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -2594,7 +2594,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2629,7 +2629,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>13</v>
       </c>
@@ -2664,7 +2664,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -2699,7 +2699,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -2734,7 +2734,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2769,7 +2769,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2804,7 +2804,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -2839,7 +2839,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -2874,7 +2874,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>15</v>
       </c>
@@ -2909,7 +2909,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>16</v>
       </c>
@@ -2944,7 +2944,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>16</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>17</v>
       </c>
@@ -3014,7 +3014,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>17</v>
       </c>
@@ -3049,7 +3049,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>18</v>
       </c>
@@ -3084,7 +3084,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -3119,7 +3119,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>19</v>
       </c>
@@ -3154,7 +3154,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>19</v>
       </c>
@@ -3189,7 +3189,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>20</v>
       </c>
@@ -3224,7 +3224,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>21</v>
       </c>
@@ -3259,7 +3259,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>21</v>
       </c>
@@ -3294,7 +3294,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>22</v>
       </c>
@@ -3329,7 +3329,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>22</v>
       </c>
@@ -3364,7 +3364,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>22</v>
       </c>
@@ -3399,7 +3399,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>22</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>23</v>
       </c>
@@ -3469,7 +3469,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>23</v>
       </c>
@@ -3504,7 +3504,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>24</v>
       </c>
@@ -3539,7 +3539,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>24</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>25</v>
       </c>
@@ -3609,7 +3609,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>25</v>
       </c>
@@ -3644,7 +3644,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>25</v>
       </c>
@@ -3679,7 +3679,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>25</v>
       </c>
@@ -3714,7 +3714,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>26</v>
       </c>
@@ -3749,7 +3749,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>26</v>
       </c>
@@ -3784,7 +3784,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>26</v>
       </c>
@@ -3819,7 +3819,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>26</v>
       </c>
@@ -3854,7 +3854,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>27</v>
       </c>
@@ -3889,7 +3889,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>27</v>
       </c>
@@ -3920,8 +3920,11 @@
       <c r="J48" t="s">
         <v>452</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K48" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>28</v>
       </c>
@@ -3956,7 +3959,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>28</v>
       </c>
@@ -3991,7 +3994,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>28</v>
       </c>
@@ -4026,7 +4029,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>28</v>
       </c>
@@ -4061,7 +4064,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>29</v>
       </c>
@@ -4096,7 +4099,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>29</v>
       </c>
@@ -4131,7 +4134,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>29</v>
       </c>
@@ -4166,7 +4169,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>29</v>
       </c>
@@ -4201,7 +4204,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>30</v>
       </c>
@@ -4236,7 +4239,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>30</v>
       </c>
@@ -4271,7 +4274,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>31</v>
       </c>
@@ -4306,7 +4309,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>31</v>
       </c>
@@ -4341,7 +4344,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>31</v>
       </c>
@@ -4376,7 +4379,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>31</v>
       </c>
@@ -4411,7 +4414,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>32</v>
       </c>
@@ -4446,7 +4449,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>32</v>
       </c>
@@ -4481,7 +4484,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>33</v>
       </c>
@@ -4516,7 +4519,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>33</v>
       </c>
@@ -4551,7 +4554,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>34</v>
       </c>
@@ -4586,7 +4589,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>34</v>
       </c>
@@ -4621,7 +4624,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>35</v>
       </c>
@@ -4656,7 +4659,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>35</v>
       </c>
@@ -4691,7 +4694,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>36</v>
       </c>
@@ -4726,7 +4729,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>36</v>
       </c>
@@ -4761,7 +4764,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>37</v>
       </c>
@@ -4796,7 +4799,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>37</v>
       </c>
@@ -4831,7 +4834,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>38</v>
       </c>
@@ -4866,7 +4869,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>39</v>
       </c>
@@ -4901,7 +4904,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>39</v>
       </c>
@@ -4936,7 +4939,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -4971,7 +4974,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>39</v>
       </c>
@@ -5006,7 +5009,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>40</v>
       </c>
@@ -5041,7 +5044,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>40</v>
       </c>
@@ -5076,7 +5079,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>41</v>
       </c>
@@ -5111,7 +5114,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>41</v>
       </c>
@@ -5146,7 +5149,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>41</v>
       </c>
@@ -5181,7 +5184,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>41</v>
       </c>
@@ -5216,7 +5219,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>42</v>
       </c>
@@ -5251,7 +5254,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>43</v>
       </c>
@@ -5286,7 +5289,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>43</v>
       </c>
@@ -5321,7 +5324,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>43</v>
       </c>
@@ -5356,7 +5359,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>43</v>
       </c>
@@ -5391,7 +5394,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>44</v>
       </c>
@@ -5426,7 +5429,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>44</v>
       </c>
@@ -5461,7 +5464,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="93" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>45</v>
       </c>
@@ -5496,7 +5499,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="94" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>45</v>
       </c>
@@ -5531,7 +5534,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="95" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>45</v>
       </c>
@@ -5566,7 +5569,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>45</v>
       </c>
@@ -5601,7 +5604,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="97" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>46</v>
       </c>
@@ -5636,7 +5639,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="98" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>46</v>
       </c>
@@ -5671,7 +5674,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="99" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>47</v>
       </c>
@@ -5706,7 +5709,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="100" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>47</v>
       </c>
@@ -5741,7 +5744,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="101" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>48</v>
       </c>
@@ -5776,7 +5779,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="102" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>48</v>
       </c>
@@ -5811,7 +5814,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="103" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>49</v>
       </c>
@@ -5846,7 +5849,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>49</v>
       </c>
@@ -5881,7 +5884,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>50</v>
       </c>
@@ -5916,7 +5919,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>50</v>
       </c>
@@ -5951,7 +5954,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="107" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>51</v>
       </c>
@@ -5986,7 +5989,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="108" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>51</v>
       </c>
@@ -6021,7 +6024,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="109" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>52</v>
       </c>
@@ -6056,7 +6059,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="110" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>52</v>
       </c>
@@ -6091,7 +6094,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="111" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>52</v>
       </c>
@@ -6126,7 +6129,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="112" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>52</v>
       </c>
@@ -6161,7 +6164,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="113" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>53</v>
       </c>
@@ -6196,7 +6199,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="114" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>53</v>
       </c>
@@ -6231,7 +6234,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="115" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>54</v>
       </c>
@@ -6266,7 +6269,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="116" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>54</v>
       </c>
@@ -6301,7 +6304,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="117" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>54</v>
       </c>
@@ -6336,7 +6339,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="118" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>54</v>
       </c>
@@ -6371,7 +6374,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="119" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>55</v>
       </c>
@@ -6406,7 +6409,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="120" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>55</v>
       </c>
@@ -6441,7 +6444,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="121" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>56</v>
       </c>
@@ -6476,7 +6479,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="122" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>56</v>
       </c>
@@ -6511,7 +6514,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="123" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>56</v>
       </c>
@@ -6546,7 +6549,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="124" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>56</v>
       </c>
@@ -6581,7 +6584,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="125" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>57</v>
       </c>
@@ -6616,7 +6619,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="126" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>57</v>
       </c>
@@ -6651,7 +6654,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="127" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>57</v>
       </c>
@@ -6686,7 +6689,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="128" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>57</v>
       </c>
@@ -6721,7 +6724,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="129" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>58</v>
       </c>
@@ -6756,7 +6759,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="130" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>58</v>
       </c>
@@ -6791,7 +6794,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="131" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>59</v>
       </c>
@@ -6826,7 +6829,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="132" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>60</v>
       </c>
@@ -6861,7 +6864,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="133" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>60</v>
       </c>
@@ -6896,7 +6899,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="134" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>61</v>
       </c>
@@ -6931,7 +6934,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="135" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>61</v>
       </c>
@@ -6966,7 +6969,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="136" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>61</v>
       </c>
@@ -7001,7 +7004,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="137" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>61</v>
       </c>
@@ -7032,8 +7035,11 @@
       <c r="J137" t="s">
         <v>484</v>
       </c>
-    </row>
-    <row r="138" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K137" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="138" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>62</v>
       </c>
@@ -7068,7 +7074,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="139" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="139" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>62</v>
       </c>
@@ -7103,7 +7109,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="140" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>63</v>
       </c>
@@ -7138,7 +7144,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="141" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>63</v>
       </c>
@@ -7173,7 +7179,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="142" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="142" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>64</v>
       </c>
@@ -7208,7 +7214,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="143" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="143" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>64</v>
       </c>
@@ -7243,7 +7249,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="144" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="144" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>65</v>
       </c>
@@ -7278,7 +7284,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="145" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="145" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>66</v>
       </c>
@@ -7313,7 +7319,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="146" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="146" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>66</v>
       </c>
@@ -7348,7 +7354,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="147" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="147" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>66</v>
       </c>
@@ -7383,7 +7389,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="148" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="148" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>67</v>
       </c>
@@ -7418,7 +7424,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="149" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="149" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>67</v>
       </c>
@@ -7453,7 +7459,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="150" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="150" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>68</v>
       </c>
@@ -7488,7 +7494,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="151" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="151" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>68</v>
       </c>
@@ -7523,7 +7529,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="152" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="152" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>69</v>
       </c>
@@ -7558,7 +7564,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="153" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="153" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>70</v>
       </c>
@@ -7593,7 +7599,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="154" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="154" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>70</v>
       </c>
@@ -7628,7 +7634,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="155" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="155" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>71</v>
       </c>
@@ -7663,7 +7669,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="156" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="156" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>71</v>
       </c>
@@ -7698,7 +7704,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="157" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="157" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>72</v>
       </c>
@@ -7733,7 +7739,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="158" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="158" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>72</v>
       </c>
@@ -7768,7 +7774,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="159" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="159" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>72</v>
       </c>
@@ -7803,7 +7809,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="160" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="160" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>73</v>
       </c>
@@ -7838,7 +7844,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="161" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="161" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>73</v>
       </c>
@@ -7873,7 +7879,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="162" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="162" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>74</v>
       </c>
@@ -7908,7 +7914,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="163" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="163" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>74</v>
       </c>
@@ -7943,7 +7949,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="164" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="164" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>75</v>
       </c>
@@ -7978,7 +7984,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="165" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="165" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>75</v>
       </c>
@@ -8013,7 +8019,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="166" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="166" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>76</v>
       </c>
@@ -8048,7 +8054,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="167" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="167" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>76</v>
       </c>
@@ -8083,7 +8089,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="168" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="168" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>76</v>
       </c>
@@ -8118,7 +8124,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="169" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="169" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>77</v>
       </c>
@@ -8153,7 +8159,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="170" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="170" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>77</v>
       </c>
@@ -8188,7 +8194,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="171" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="171" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>77</v>
       </c>
@@ -8223,7 +8229,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="172" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="172" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>77</v>
       </c>
@@ -8258,7 +8264,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="173" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="173" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>78</v>
       </c>
@@ -8293,7 +8299,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="174" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="174" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>78</v>
       </c>
@@ -8328,7 +8334,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="175" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="175" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>79</v>
       </c>
@@ -8363,7 +8369,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="176" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="176" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>79</v>
       </c>
@@ -8398,7 +8404,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="177" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="177" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>80</v>
       </c>
@@ -8433,7 +8439,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="178" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="178" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>80</v>
       </c>
@@ -8468,7 +8474,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="179" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="179" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>81</v>
       </c>
@@ -8503,7 +8509,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="180" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="180" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>82</v>
       </c>
@@ -8538,7 +8544,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="181" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="181" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>82</v>
       </c>
@@ -8573,7 +8579,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="182" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="182" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>83</v>
       </c>
@@ -8608,7 +8614,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="183" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="183" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>83</v>
       </c>
@@ -8643,7 +8649,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="184" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="184" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>84</v>
       </c>
@@ -8678,7 +8684,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="185" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="185" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>84</v>
       </c>
@@ -8713,7 +8719,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="186" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="186" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>85</v>
       </c>
@@ -8748,7 +8754,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="187" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="187" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>85</v>
       </c>
@@ -8783,7 +8789,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="188" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="188" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>86</v>
       </c>
@@ -8818,7 +8824,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="189" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="189" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>86</v>
       </c>
@@ -8853,7 +8859,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="190" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="190" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>87</v>
       </c>
@@ -8888,7 +8894,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="191" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="191" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>87</v>
       </c>
@@ -8923,7 +8929,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="192" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="192" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>88</v>
       </c>
@@ -8958,7 +8964,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="193" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="193" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>88</v>
       </c>
@@ -8993,7 +8999,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="194" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="194" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>88</v>
       </c>
@@ -9028,7 +9034,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="195" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="195" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>88</v>
       </c>
@@ -9063,7 +9069,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="196" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="196" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>89</v>
       </c>
@@ -9098,7 +9104,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="197" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="197" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>89</v>
       </c>
@@ -9133,7 +9139,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="198" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="198" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>89</v>
       </c>
@@ -9168,7 +9174,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="199" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="199" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>89</v>
       </c>
@@ -9203,7 +9209,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="200" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="200" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>90</v>
       </c>
@@ -9238,7 +9244,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="201" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="201" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>90</v>
       </c>
@@ -9273,7 +9279,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="202" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="202" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>91</v>
       </c>
@@ -9308,7 +9314,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="203" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="203" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>91</v>
       </c>
@@ -9343,7 +9349,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="204" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="204" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>92</v>
       </c>
@@ -9378,7 +9384,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="205" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="205" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>92</v>
       </c>
@@ -9413,7 +9419,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="206" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="206" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>93</v>
       </c>
@@ -9448,7 +9454,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="207" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="207" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>93</v>
       </c>
@@ -9483,7 +9489,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="208" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="208" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>94</v>
       </c>
@@ -9518,7 +9524,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="209" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="209" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>95</v>
       </c>
@@ -9553,7 +9559,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="210" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="210" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>95</v>
       </c>
@@ -9588,7 +9594,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="211" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="211" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>95</v>
       </c>
@@ -9623,7 +9629,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="212" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="212" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>95</v>
       </c>
@@ -9658,7 +9664,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="213" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="213" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>96</v>
       </c>
@@ -9693,7 +9699,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="214" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="214" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>96</v>
       </c>
@@ -9728,7 +9734,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="215" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="215" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>96</v>
       </c>
@@ -9763,7 +9769,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="216" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="216" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>96</v>
       </c>
@@ -9798,7 +9804,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="217" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="217" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>97</v>
       </c>
@@ -9833,7 +9839,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="218" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="218" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>97</v>
       </c>
@@ -9864,8 +9870,11 @@
       <c r="J218" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="219" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="K218" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="219" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>98</v>
       </c>
@@ -9900,7 +9909,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="220" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="220" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>98</v>
       </c>
@@ -9935,7 +9944,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="221" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="221" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>99</v>
       </c>
@@ -9970,7 +9979,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="222" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="222" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>99</v>
       </c>
@@ -10005,7 +10014,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="223" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="223" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>100</v>
       </c>
@@ -10040,7 +10049,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="224" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="224" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>100</v>
       </c>
@@ -10075,7 +10084,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="225" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="225" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>101</v>
       </c>
@@ -10110,7 +10119,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="226" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="226" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>101</v>
       </c>
@@ -10145,7 +10154,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="227" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="227" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>102</v>
       </c>
@@ -10180,7 +10189,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="228" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="228" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>102</v>
       </c>
@@ -10215,7 +10224,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="229" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="229" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>103</v>
       </c>
@@ -10250,7 +10259,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="230" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="230" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>103</v>
       </c>
@@ -10285,7 +10294,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="231" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="231" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>104</v>
       </c>
@@ -10320,7 +10329,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="232" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="232" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>104</v>
       </c>
@@ -10355,7 +10364,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="233" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="233" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>105</v>
       </c>
@@ -10390,7 +10399,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="234" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="234" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>106</v>
       </c>
@@ -10425,7 +10434,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="235" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="235" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>106</v>
       </c>
@@ -10460,7 +10469,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="236" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="236" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>106</v>
       </c>
@@ -10495,7 +10504,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="237" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="237" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>107</v>
       </c>
@@ -10530,7 +10539,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="238" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="238" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>107</v>
       </c>
@@ -10565,7 +10574,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="239" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="239" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>107</v>
       </c>
@@ -10600,7 +10609,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="240" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="240" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>107</v>
       </c>
@@ -10635,7 +10644,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="241" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="241" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>108</v>
       </c>
@@ -10670,7 +10679,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="242" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="242" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>108</v>
       </c>
@@ -10705,7 +10714,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="243" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="243" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>109</v>
       </c>
@@ -10740,7 +10749,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="244" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="244" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>109</v>
       </c>
@@ -10775,7 +10784,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="245" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="245" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>110</v>
       </c>
@@ -10810,7 +10819,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="246" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="246" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>110</v>
       </c>
@@ -10845,7 +10854,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="247" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="247" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>110</v>
       </c>
@@ -10880,7 +10889,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="248" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="248" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>110</v>
       </c>
@@ -10915,7 +10924,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="249" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="249" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>111</v>
       </c>
@@ -10950,7 +10959,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="250" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="250" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>111</v>
       </c>
@@ -10985,7 +10994,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="251" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="251" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>112</v>
       </c>
@@ -11020,7 +11029,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="252" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="252" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>112</v>
       </c>
@@ -11055,7 +11064,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="253" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="253" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>113</v>
       </c>
@@ -11090,7 +11099,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="254" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="254" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>113</v>
       </c>
@@ -11125,7 +11134,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="255" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="255" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>113</v>
       </c>
@@ -11160,7 +11169,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="256" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="256" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>113</v>
       </c>
@@ -11195,7 +11204,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="257" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="257" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>114</v>
       </c>
@@ -11230,7 +11239,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="258" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="258" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>114</v>
       </c>
@@ -11265,7 +11274,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="259" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="259" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>114</v>
       </c>
@@ -11300,7 +11309,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="260" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="260" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>114</v>
       </c>
@@ -11335,7 +11344,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="261" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="261" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A261" t="s">
         <v>115</v>
       </c>
@@ -11370,7 +11379,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="262" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="262" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A262" t="s">
         <v>115</v>
       </c>
@@ -11405,7 +11414,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="263" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="263" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A263" t="s">
         <v>115</v>
       </c>
@@ -11440,7 +11449,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="264" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="264" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A264" t="s">
         <v>115</v>
       </c>
@@ -11475,7 +11484,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="265" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="265" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A265" t="s">
         <v>116</v>
       </c>
@@ -11510,7 +11519,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="266" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="266" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A266" t="s">
         <v>116</v>
       </c>
@@ -11545,7 +11554,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="267" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="267" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A267" t="s">
         <v>117</v>
       </c>
@@ -11580,7 +11589,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="268" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="268" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A268" t="s">
         <v>117</v>
       </c>
@@ -11615,7 +11624,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="269" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="269" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A269" t="s">
         <v>118</v>
       </c>
@@ -11650,7 +11659,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="270" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="270" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A270" t="s">
         <v>118</v>
       </c>
@@ -11685,7 +11694,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="271" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="271" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A271" t="s">
         <v>118</v>
       </c>
@@ -11720,7 +11729,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="272" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="272" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A272" t="s">
         <v>118</v>
       </c>
@@ -11755,7 +11764,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="273" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="273" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A273" t="s">
         <v>119</v>
       </c>
@@ -11790,7 +11799,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="274" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="274" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A274" t="s">
         <v>119</v>
       </c>
@@ -11825,7 +11834,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="275" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="275" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A275" t="s">
         <v>120</v>
       </c>
@@ -11860,7 +11869,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="276" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="276" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A276" t="s">
         <v>120</v>
       </c>
@@ -11895,7 +11904,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="277" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="277" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A277" t="s">
         <v>121</v>
       </c>
@@ -11930,7 +11939,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="278" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="278" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A278" t="s">
         <v>121</v>
       </c>
@@ -11965,7 +11974,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="279" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="279" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A279" t="s">
         <v>121</v>
       </c>
@@ -12000,7 +12009,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="280" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="280" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A280" t="s">
         <v>121</v>
       </c>
@@ -12035,7 +12044,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="281" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="281" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A281" t="s">
         <v>122</v>
       </c>
@@ -12070,7 +12079,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="282" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="282" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A282" t="s">
         <v>122</v>
       </c>
@@ -12105,7 +12114,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="283" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="283" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A283" t="s">
         <v>123</v>
       </c>
@@ -12140,7 +12149,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="284" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="284" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A284" t="s">
         <v>123</v>
       </c>
@@ -12175,7 +12184,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="285" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="285" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A285" t="s">
         <v>124</v>
       </c>
@@ -12210,7 +12219,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="286" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="286" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A286" t="s">
         <v>124</v>
       </c>
@@ -12245,7 +12254,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="287" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="287" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A287" t="s">
         <v>124</v>
       </c>
@@ -12280,7 +12289,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="288" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="288" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A288" t="s">
         <v>124</v>
       </c>
@@ -12315,7 +12324,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="289" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="289" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A289" t="s">
         <v>125</v>
       </c>
@@ -12350,7 +12359,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="290" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="290" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A290" t="s">
         <v>125</v>
       </c>
@@ -12385,7 +12394,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="291" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="291" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A291" t="s">
         <v>125</v>
       </c>
@@ -12420,7 +12429,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="292" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="292" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A292" t="s">
         <v>125</v>
       </c>
@@ -12455,7 +12464,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="293" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="293" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A293" t="s">
         <v>126</v>
       </c>
@@ -12490,7 +12499,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="294" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="294" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A294" t="s">
         <v>126</v>
       </c>
@@ -12525,7 +12534,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="295" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="295" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A295" t="s">
         <v>127</v>
       </c>
@@ -12560,7 +12569,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="296" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="296" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A296" t="s">
         <v>128</v>
       </c>
@@ -12595,7 +12604,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="297" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="297" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A297" t="s">
         <v>128</v>
       </c>
@@ -12630,7 +12639,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="298" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="298" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A298" t="s">
         <v>129</v>
       </c>
@@ -12665,7 +12674,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="299" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="299" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A299" t="s">
         <v>129</v>
       </c>
@@ -12700,7 +12709,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="300" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="300" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A300" t="s">
         <v>129</v>
       </c>
@@ -12735,7 +12744,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="301" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="301" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A301" t="s">
         <v>129</v>
       </c>
@@ -12770,7 +12779,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="302" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="302" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A302" t="s">
         <v>130</v>
       </c>
@@ -12805,7 +12814,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="303" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="303" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A303" t="s">
         <v>130</v>
       </c>
@@ -12840,7 +12849,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="304" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="304" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A304" t="s">
         <v>131</v>
       </c>
@@ -12875,7 +12884,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="305" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="305" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A305" t="s">
         <v>131</v>
       </c>
@@ -12910,7 +12919,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="306" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="306" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A306" t="s">
         <v>132</v>
       </c>
@@ -12945,7 +12954,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="307" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="307" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A307" t="s">
         <v>132</v>
       </c>
@@ -12980,7 +12989,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="308" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="308" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A308" t="s">
         <v>132</v>
       </c>
@@ -13015,7 +13024,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="309" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="309" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A309" t="s">
         <v>132</v>
       </c>
@@ -13050,7 +13059,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="310" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="310" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A310" t="s">
         <v>133</v>
       </c>
@@ -13085,7 +13094,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="311" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="311" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A311" t="s">
         <v>133</v>
       </c>
@@ -13120,7 +13129,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="312" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="312" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A312" t="s">
         <v>134</v>
       </c>
@@ -13155,7 +13164,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="313" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="313" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A313" t="s">
         <v>135</v>
       </c>
@@ -13190,7 +13199,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="314" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="314" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A314" t="s">
         <v>135</v>
       </c>
@@ -13225,7 +13234,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="315" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="315" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A315" t="s">
         <v>136</v>
       </c>
@@ -13260,7 +13269,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="316" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="316" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A316" t="s">
         <v>136</v>
       </c>
@@ -13295,7 +13304,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="317" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="317" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A317" t="s">
         <v>137</v>
       </c>
@@ -13330,7 +13339,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="318" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="318" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A318" t="s">
         <v>137</v>
       </c>
@@ -13365,7 +13374,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="319" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="319" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A319" t="s">
         <v>138</v>
       </c>
@@ -13400,7 +13409,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="320" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="320" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A320" t="s">
         <v>138</v>
       </c>
@@ -13435,7 +13444,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="321" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="321" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A321" t="s">
         <v>139</v>
       </c>
@@ -13470,7 +13479,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="322" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="322" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A322" t="s">
         <v>139</v>
       </c>
@@ -13505,7 +13514,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="323" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="323" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A323" t="s">
         <v>140</v>
       </c>
@@ -13540,7 +13549,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="324" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="324" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A324" t="s">
         <v>140</v>
       </c>
@@ -13575,7 +13584,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="325" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="325" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A325" t="s">
         <v>141</v>
       </c>
@@ -13610,7 +13619,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="326" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="326" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A326" t="s">
         <v>141</v>
       </c>
@@ -13645,7 +13654,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="327" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="327" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A327" t="s">
         <v>141</v>
       </c>
@@ -13680,7 +13689,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="328" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="328" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A328" t="s">
         <v>141</v>
       </c>
@@ -13715,7 +13724,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="329" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="329" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A329" t="s">
         <v>142</v>
       </c>
@@ -13750,7 +13759,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="330" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="330" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A330" t="s">
         <v>142</v>
       </c>
@@ -13785,7 +13794,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="331" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="331" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A331" t="s">
         <v>143</v>
       </c>
@@ -13820,7 +13829,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="332" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="332" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A332" t="s">
         <v>143</v>
       </c>
@@ -13855,7 +13864,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="333" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="333" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A333" t="s">
         <v>144</v>
       </c>
@@ -13890,7 +13899,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="334" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="334" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A334" t="s">
         <v>144</v>
       </c>
@@ -13925,7 +13934,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="335" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="335" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A335" t="s">
         <v>145</v>
       </c>
@@ -13960,7 +13969,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="336" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="336" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A336" t="s">
         <v>145</v>
       </c>
@@ -13995,7 +14004,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="337" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="337" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A337" t="s">
         <v>145</v>
       </c>
@@ -14030,7 +14039,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="338" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="338" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A338" t="s">
         <v>145</v>
       </c>
@@ -14065,7 +14074,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="339" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="339" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A339" t="s">
         <v>146</v>
       </c>
@@ -14100,7 +14109,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="340" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="340" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A340" t="s">
         <v>146</v>
       </c>
@@ -14135,7 +14144,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="341" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="341" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A341" t="s">
         <v>147</v>
       </c>
@@ -14170,7 +14179,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="342" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="342" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A342" t="s">
         <v>147</v>
       </c>
@@ -14205,7 +14214,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="343" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="343" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A343" t="s">
         <v>148</v>
       </c>
@@ -14240,7 +14249,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="344" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="344" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A344" t="s">
         <v>149</v>
       </c>
@@ -14275,7 +14284,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="345" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="345" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A345" t="s">
         <v>149</v>
       </c>
@@ -14310,7 +14319,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="346" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="346" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A346" t="s">
         <v>150</v>
       </c>
@@ -14345,7 +14354,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="347" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="347" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A347" t="s">
         <v>151</v>
       </c>
@@ -14380,7 +14389,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="348" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="348" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A348" t="s">
         <v>151</v>
       </c>
@@ -14415,7 +14424,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="349" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="349" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A349" t="s">
         <v>152</v>
       </c>
@@ -14450,7 +14459,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="350" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="350" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A350" t="s">
         <v>153</v>
       </c>
@@ -14485,7 +14494,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="351" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="351" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A351" t="s">
         <v>153</v>
       </c>
@@ -14520,7 +14529,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="352" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="352" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A352" t="s">
         <v>154</v>
       </c>
@@ -14555,7 +14564,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="353" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="353" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A353" t="s">
         <v>155</v>
       </c>
@@ -14590,7 +14599,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="354" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="354" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A354" t="s">
         <v>155</v>
       </c>
@@ -14625,7 +14634,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="355" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="355" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A355" t="s">
         <v>155</v>
       </c>
@@ -14660,7 +14669,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="356" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="356" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A356" t="s">
         <v>156</v>
       </c>
@@ -14695,7 +14704,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="357" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="357" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A357" t="s">
         <v>157</v>
       </c>
@@ -14730,7 +14739,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="358" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="358" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A358" t="s">
         <v>157</v>
       </c>
@@ -14765,7 +14774,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="359" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="359" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A359" t="s">
         <v>158</v>
       </c>
@@ -14800,7 +14809,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="360" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="360" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A360" t="s">
         <v>158</v>
       </c>
@@ -14835,7 +14844,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="361" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="361" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A361" t="s">
         <v>159</v>
       </c>
@@ -14870,7 +14879,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="362" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="362" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A362" t="s">
         <v>159</v>
       </c>
@@ -14905,7 +14914,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="363" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="363" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A363" t="s">
         <v>159</v>
       </c>
@@ -14940,7 +14949,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="364" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="364" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A364" t="s">
         <v>159</v>
       </c>
@@ -14975,7 +14984,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="365" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="365" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A365" t="s">
         <v>160</v>
       </c>
@@ -15010,7 +15019,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="366" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="366" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A366" t="s">
         <v>160</v>
       </c>
@@ -15045,7 +15054,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="367" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="367" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A367" t="s">
         <v>161</v>
       </c>
@@ -15080,7 +15089,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="368" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="368" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A368" t="s">
         <v>161</v>
       </c>
@@ -15115,7 +15124,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="369" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="369" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A369" t="s">
         <v>161</v>
       </c>
@@ -15150,7 +15159,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="370" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="370" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A370" t="s">
         <v>161</v>
       </c>
@@ -15185,7 +15194,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="371" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="371" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A371" t="s">
         <v>162</v>
       </c>
@@ -15220,7 +15229,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="372" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="372" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A372" t="s">
         <v>162</v>
       </c>
@@ -15255,7 +15264,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="373" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="373" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A373" t="s">
         <v>163</v>
       </c>
@@ -15290,7 +15299,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="374" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="374" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A374" t="s">
         <v>163</v>
       </c>
@@ -15325,7 +15334,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="375" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="375" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A375" t="s">
         <v>164</v>
       </c>
@@ -15360,7 +15369,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="376" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="376" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A376" t="s">
         <v>164</v>
       </c>
@@ -15395,7 +15404,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="377" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="377" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A377" t="s">
         <v>164</v>
       </c>
@@ -15430,7 +15439,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="378" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="378" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A378" t="s">
         <v>164</v>
       </c>
@@ -15465,7 +15474,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="379" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="379" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A379" t="s">
         <v>165</v>
       </c>
@@ -15500,7 +15509,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="380" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="380" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A380" t="s">
         <v>165</v>
       </c>
@@ -15535,7 +15544,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="381" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="381" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A381" t="s">
         <v>165</v>
       </c>
@@ -15570,7 +15579,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="382" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="382" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A382" t="s">
         <v>166</v>
       </c>
@@ -15605,7 +15614,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="383" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="383" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A383" t="s">
         <v>166</v>
       </c>
@@ -15640,7 +15649,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="384" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="384" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A384" t="s">
         <v>166</v>
       </c>
@@ -15675,7 +15684,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="385" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="385" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A385" t="s">
         <v>166</v>
       </c>
@@ -15710,7 +15719,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="386" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="386" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A386" t="s">
         <v>167</v>
       </c>
@@ -15745,7 +15754,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="387" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="387" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A387" t="s">
         <v>167</v>
       </c>
@@ -15780,7 +15789,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="388" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="388" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A388" t="s">
         <v>168</v>
       </c>
@@ -15815,7 +15824,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="389" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="389" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A389" t="s">
         <v>168</v>
       </c>
@@ -15850,7 +15859,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="390" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="390" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A390" t="s">
         <v>169</v>
       </c>
@@ -15885,7 +15894,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="391" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="391" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A391" t="s">
         <v>169</v>
       </c>
@@ -15920,7 +15929,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="392" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="392" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A392" t="s">
         <v>170</v>
       </c>
@@ -15955,7 +15964,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="393" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="393" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A393" t="s">
         <v>170</v>
       </c>

</xml_diff>